<commit_message>
Add upload file to create project
</commit_message>
<xml_diff>
--- a/uploads/file.xlsx
+++ b/uploads/file.xlsx
@@ -129,36 +129,8 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -470,7 +442,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -560,7 +532,7 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -601,7 +573,7 @@
         <v>1</v>
       </c>
       <c r="M3">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -642,7 +614,7 @@
         <v>1</v>
       </c>
       <c r="M4">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -683,7 +655,7 @@
         <v>1</v>
       </c>
       <c r="M5">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -724,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="M6">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -765,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="M7">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -806,7 +778,7 @@
         <v>1</v>
       </c>
       <c r="M8">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -847,7 +819,7 @@
         <v>1</v>
       </c>
       <c r="M9">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -888,7 +860,7 @@
         <v>1</v>
       </c>
       <c r="M10">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -929,7 +901,7 @@
         <v>1</v>
       </c>
       <c r="M11">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -970,7 +942,7 @@
         <v>1</v>
       </c>
       <c r="M12">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1011,7 +983,7 @@
         <v>1</v>
       </c>
       <c r="M13">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1052,7 +1024,7 @@
         <v>1</v>
       </c>
       <c r="M14">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1093,7 +1065,7 @@
         <v>1</v>
       </c>
       <c r="M15">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1134,7 +1106,7 @@
         <v>1</v>
       </c>
       <c r="M16">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1175,7 +1147,7 @@
         <v>1</v>
       </c>
       <c r="M17">
-        <v>9999999</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change the readme file for software function.
</commit_message>
<xml_diff>
--- a/uploads/file.xlsx
+++ b/uploads/file.xlsx
@@ -1,95 +1,77 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hxxu/Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>project_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>building</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>unit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>floor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>position</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>width</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>height</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>is_stored</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>product_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>created_at</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>updated_at</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>框</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -113,48 +95,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -177,7 +131,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -189,7 +143,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -208,7 +162,7 @@
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -243,7 +197,7 @@
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -423,15 +377,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,66 +410,86 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>9</v>
-      </c>
-      <c r="E2">
-        <v>9</v>
-      </c>
-      <c r="F2">
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <v>9</v>
-      </c>
-      <c r="H2">
-        <v>9</v>
-      </c>
-      <c r="I2">
-        <v>9</v>
-      </c>
-      <c r="J2">
-        <v>9</v>
-      </c>
-      <c r="K2">
-        <v>9</v>
-      </c>
-      <c r="L2">
-        <v>9</v>
-      </c>
-      <c r="M2">
-        <v>9</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1">
+        <v>7</v>
+      </c>
+      <c r="H4" s="1">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>